<commit_message>
Atualização Fases Liberta e Sula
</commit_message>
<xml_diff>
--- a/libertadores/datasets_liberta/classificacao_por_grupo_fase_3.xlsx
+++ b/libertadores/datasets_liberta/classificacao_por_grupo_fase_3.xlsx
@@ -498,13 +498,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1216.37109375</v>
+        <v>118.740234375</v>
       </c>
       <c r="H2">
         <v>106.2099609375</v>
       </c>
       <c r="I2">
-        <v>1110.1611328125</v>
+        <v>12.5302734375</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -530,13 +530,13 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1044.509765625</v>
+        <v>106.2099609375</v>
       </c>
       <c r="H3">
         <v>118.740234375</v>
       </c>
       <c r="I3">
-        <v>925.76953125</v>
+        <v>-12.5302734375</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -607,13 +607,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1158.7392578125</v>
+        <v>111.91015625</v>
       </c>
       <c r="H2">
         <v>93.509765625</v>
       </c>
       <c r="I2">
-        <v>1065.2294921875</v>
+        <v>18.400390625</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -639,13 +639,13 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1155.5400390625</v>
+        <v>93.509765625</v>
       </c>
       <c r="H3">
         <v>111.91015625</v>
       </c>
       <c r="I3">
-        <v>1043.6298828125</v>
+        <v>-18.400390625</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -716,13 +716,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1022.77978515625</v>
+        <v>111.10986328125</v>
       </c>
       <c r="H2">
         <v>103.81005859375</v>
       </c>
       <c r="I2">
-        <v>918.9697265625</v>
+        <v>7.2998046875</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -748,13 +748,13 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1163.760009765625</v>
+        <v>103.81005859375</v>
       </c>
       <c r="H3">
         <v>111.10986328125</v>
       </c>
       <c r="I3">
-        <v>1052.650146484375</v>
+        <v>-7.2998046875</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -825,13 +825,13 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1060.820434570312</v>
+        <v>120.25</v>
       </c>
       <c r="H2">
         <v>111.2099609375</v>
       </c>
       <c r="I2">
-        <v>949.6104736328125</v>
+        <v>9.0400390625</v>
       </c>
       <c r="J2">
         <v>1</v>
@@ -857,13 +857,13 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1155.240234375</v>
+        <v>111.2099609375</v>
       </c>
       <c r="H3">
         <v>120.25</v>
       </c>
       <c r="I3">
-        <v>1034.990234375</v>
+        <v>-9.0400390625</v>
       </c>
       <c r="J3">
         <v>2</v>

</xml_diff>